<commit_message>
Updated results of SP Class B
</commit_message>
<xml_diff>
--- a/code/results/energy_estimation/energy.xlsx
+++ b/code/results/energy_estimation/energy.xlsx
@@ -383,10 +383,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>477521.1715133165</v>
+        <v>3002.821152451515</v>
       </c>
       <c r="C2" t="n">
-        <v>473897.9420047742</v>
+        <v>3300.800374378629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results of SP Class D
</commit_message>
<xml_diff>
--- a/code/results/energy_estimation/energy.xlsx
+++ b/code/results/energy_estimation/energy.xlsx
@@ -383,10 +383,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3002.821152451515</v>
+        <v>289994.3270374199</v>
       </c>
       <c r="C2" t="n">
-        <v>3300.800374378629</v>
+        <v>325460.6920583829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results SP-D parallel execution
</commit_message>
<xml_diff>
--- a/code/results/energy_estimation/energy.xlsx
+++ b/code/results/energy_estimation/energy.xlsx
@@ -383,10 +383,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>289994.3270374199</v>
+        <v>332458.6269462494</v>
       </c>
       <c r="C2" t="n">
-        <v>325460.6920583829</v>
+        <v>355812.1745885832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed results of SP-D to new directory
</commit_message>
<xml_diff>
--- a/code/results/energy_estimation/energy.xlsx
+++ b/code/results/energy_estimation/energy.xlsx
@@ -383,10 +383,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>332458.6269462494</v>
+        <v>331941.8095985432</v>
       </c>
       <c r="C2" t="n">
-        <v>355812.1745885832</v>
+        <v>355260.6399736041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>